<commit_message>
ID 3 AB, calcualted diff of lag 7 and avg of lags 2,3,and 4
</commit_message>
<xml_diff>
--- a/Code/(11)/Acc_final_Placebo.xlsx
+++ b/Code/(11)/Acc_final_Placebo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="13" documentId="8_{46BC5A2B-194E-4571-B6C2-E5D41A72B66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B025E51-F137-4672-8B6D-EC9EF1A248E7}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{7EEE1518-5726-4AEC-9A9A-6CBBEC7CB3C7}"/>
+    <workbookView xWindow="10050" yWindow="2295" windowWidth="21600" windowHeight="12645" xr2:uid="{7EEE1518-5726-4AEC-9A9A-6CBBEC7CB3C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Placebo" sheetId="1" r:id="rId1"/>
@@ -127,10 +127,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A4FAF9-D9AE-406E-9D70-8F06AFB8588A}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>